<commit_message>
add grid search trial
</commit_message>
<xml_diff>
--- a/Analysis/CrowdData/pilot_aggregates_part1_analysis.xlsx
+++ b/Analysis/CrowdData/pilot_aggregates_part1_analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="pivot" sheetId="2" r:id="rId1"/>
@@ -26,16 +26,16 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId9"/>
-    <pivotCache cacheId="3" r:id="rId10"/>
-    <pivotCache cacheId="4" r:id="rId11"/>
-    <pivotCache cacheId="11" r:id="rId12"/>
+    <pivotCache cacheId="4" r:id="rId9"/>
+    <pivotCache cacheId="5" r:id="rId10"/>
+    <pivotCache cacheId="6" r:id="rId11"/>
+    <pivotCache cacheId="7" r:id="rId12"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1990" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="838">
   <si>
     <t>img_id</t>
   </si>
@@ -2543,6 +2543,12 @@
   </si>
   <si>
     <t>val</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t># images</t>
   </si>
 </sst>
 </file>
@@ -3333,6 +3339,415 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Class Distribution</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Validation Dataset</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>val_dataset2!$K$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># images</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>val_dataset2!$K$30:$K$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3F9C-4460-8500-18168AE7294E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="568023464"/>
+        <c:axId val="568020840"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="568023464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Class</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="568020840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="568020840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># images</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="568023464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
               <a:lnSpc>
                 <a:spcPct val="100000"/>
@@ -3726,7 +4141,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6495,6 +6910,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7038,6 +7493,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7557,6 +8515,47 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B71616A4-A958-4FA2-8BB1-E5541EB98913}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -20745,7 +21744,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -20811,7 +21810,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="E1:F6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" subtotalTop="0" showAll="0">
@@ -20863,7 +21862,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J1:K7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -20922,7 +21921,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J1:K7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -57592,8 +58591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29:K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57964,7 +58963,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>84</v>
       </c>
@@ -57984,7 +58983,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>85</v>
       </c>
@@ -58004,7 +59003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>86</v>
       </c>
@@ -58024,7 +59023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>87</v>
       </c>
@@ -58044,7 +59043,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>88</v>
       </c>
@@ -58064,7 +59063,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>89</v>
       </c>
@@ -58084,7 +59083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>90</v>
       </c>
@@ -58104,7 +59103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>91</v>
       </c>
@@ -58124,7 +59123,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>92</v>
       </c>
@@ -58144,7 +59143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>93</v>
       </c>
@@ -58164,7 +59163,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>94</v>
       </c>
@@ -58184,7 +59183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>95</v>
       </c>
@@ -58204,7 +59203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>96</v>
       </c>
@@ -58223,8 +59222,14 @@
       <c r="F29" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>836</v>
+      </c>
+      <c r="K29" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>97</v>
       </c>
@@ -58243,8 +59248,14 @@
       <c r="F30" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>98</v>
       </c>
@@ -58263,8 +59274,14 @@
       <c r="F31" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="K31">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>99</v>
       </c>
@@ -58283,8 +59300,14 @@
       <c r="F32" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J32">
+        <v>3</v>
+      </c>
+      <c r="K32">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>100</v>
       </c>
@@ -58303,8 +59326,14 @@
       <c r="F33" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <v>4</v>
+      </c>
+      <c r="K33">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>101</v>
       </c>
@@ -58323,8 +59352,14 @@
       <c r="F34" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <v>5</v>
+      </c>
+      <c r="K34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>102</v>
       </c>
@@ -58344,7 +59379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>103</v>
       </c>
@@ -58364,7 +59399,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>104</v>
       </c>
@@ -58384,7 +59419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>105</v>
       </c>
@@ -58404,7 +59439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>106</v>
       </c>
@@ -58424,7 +59459,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>107</v>
       </c>
@@ -58444,7 +59479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>108</v>
       </c>
@@ -58464,7 +59499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>13</v>
       </c>
@@ -58484,7 +59519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
         <v>14</v>
       </c>
@@ -58504,7 +59539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>15</v>
       </c>
@@ -58524,7 +59559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="10">
         <v>16</v>
       </c>
@@ -58544,7 +59579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>109</v>
       </c>
@@ -58564,7 +59599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="10">
         <v>110</v>
       </c>
@@ -58584,7 +59619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>111</v>
       </c>
@@ -60866,6 +61901,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add expansion view linear and same
</commit_message>
<xml_diff>
--- a/Analysis/CrowdData/pilot_aggregates_part1_analysis.xlsx
+++ b/Analysis/CrowdData/pilot_aggregates_part1_analysis.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="pivot" sheetId="2" r:id="rId1"/>
@@ -26,16 +26,16 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId9"/>
-    <pivotCache cacheId="5" r:id="rId10"/>
-    <pivotCache cacheId="6" r:id="rId11"/>
-    <pivotCache cacheId="7" r:id="rId12"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
+    <pivotCache cacheId="1" r:id="rId10"/>
+    <pivotCache cacheId="2" r:id="rId11"/>
+    <pivotCache cacheId="3" r:id="rId12"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1993" uniqueCount="839">
   <si>
     <t>img_id</t>
   </si>
@@ -2549,12 +2549,18 @@
   </si>
   <si>
     <t># images</t>
+  </si>
+  <si>
+    <t>percentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0"/>
+  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3135,7 +3141,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3153,6 +3159,7 @@
     <xf numFmtId="0" fontId="13" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3776,12 +3783,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Label Aggregation Statistics (Image)</a:t>
+              <a:t>Label Aggregation Statistics (Image Level)</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US">
+            <a:endParaRPr lang="en-US" sz="1400">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -3853,7 +3860,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3861,6 +3868,229 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{7B0899D9-F729-4321-AC84-F63DEA3CDAD7}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-990F-44C4-B480-CF9CB13D1A8D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{9BBE98F0-4B4B-460D-88CE-2F32262F078F}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-990F-44C4-B480-CF9CB13D1A8D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{DB45818C-3873-4298-96C1-DF7B73ED17CC}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-990F-44C4-B480-CF9CB13D1A8D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{62281672-5C89-4418-B901-3E920974E76C}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-990F-44C4-B480-CF9CB13D1A8D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{0B10B76D-7FB7-495E-80C4-11483474259F}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-990F-44C4-B480-CF9CB13D1A8D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="700" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>graphs!$B$3:$B$7</c:f>
@@ -3886,6 +4116,29 @@
             </c:numRef>
           </c:val>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>graphs!$C$3:$C$7</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>2.5%</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>35.3%</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>38.5%</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>23.2%</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.5%</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-CB9E-4D3C-AAF2-105675C204EA}"/>
             </c:ext>
@@ -4189,12 +4442,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Variance of each image label (sorted)</a:t>
+              <a:t>Variance of each image attractiveness label (sorted)</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US">
+            <a:endParaRPr lang="en-US" sz="1400">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -6725,6 +6978,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>images</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> ordered by variance of attractiveness votes</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6766,6 +7079,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickLblSkip val="30"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
@@ -6789,6 +7103,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>variance</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -8556,16 +8925,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8593,13 +8962,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>300037</xdr:colOff>
+      <xdr:colOff>300036</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
@@ -21744,7 +22113,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -21810,7 +22179,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="E1:F6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" subtotalTop="0" showAll="0">
@@ -21862,7 +22231,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J1:K7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -21921,7 +22290,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J1:K7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -22353,8 +22722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58591,8 +58960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29:K34"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61910,7 +62279,7 @@
   <dimension ref="A1:K141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67706,8 +68075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P806"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67724,6 +68093,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>838</v>
+      </c>
       <c r="P2">
         <v>0</v>
       </c>
@@ -67735,6 +68107,10 @@
       <c r="B3" s="4">
         <v>20</v>
       </c>
+      <c r="C3" s="15" t="str">
+        <f>ROUND(B3/SUM($B$3:$B$7)*100,1)&amp;"%"</f>
+        <v>2.5%</v>
+      </c>
       <c r="P3">
         <v>0</v>
       </c>
@@ -67746,6 +68122,10 @@
       <c r="B4" s="4">
         <v>284</v>
       </c>
+      <c r="C4" s="15" t="str">
+        <f t="shared" ref="C4:C7" si="0">ROUND(B4/SUM($B$3:$B$7)*100,1)&amp;"%"</f>
+        <v>35.3%</v>
+      </c>
       <c r="P4">
         <v>0</v>
       </c>
@@ -67756,6 +68136,10 @@
       </c>
       <c r="B5" s="4">
         <v>310</v>
+      </c>
+      <c r="C5" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>38.5%</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -67768,6 +68152,10 @@
       <c r="B6" s="4">
         <v>187</v>
       </c>
+      <c r="C6" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>23.2%</v>
+      </c>
       <c r="P6">
         <v>0</v>
       </c>
@@ -67778,6 +68166,10 @@
       </c>
       <c r="B7" s="4">
         <v>4</v>
+      </c>
+      <c r="C7" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>0.5%</v>
       </c>
       <c r="P7">
         <v>0</v>

</xml_diff>

<commit_message>
add feature extraction CNN
</commit_message>
<xml_diff>
--- a/Analysis/CrowdData/pilot_aggregates_part1_analysis.xlsx
+++ b/Analysis/CrowdData/pilot_aggregates_part1_analysis.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="pivot" sheetId="2" r:id="rId1"/>
@@ -22,9 +22,9 @@
   </sheets>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId8"/>
-    <pivotCache cacheId="9" r:id="rId9"/>
-    <pivotCache cacheId="20" r:id="rId10"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId9"/>
+    <pivotCache cacheId="2" r:id="rId10"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -3198,25 +3198,6 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -3279,6 +3260,25 @@
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -3458,7 +3458,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B20CA9E6-4EEB-4F9F-9944-F6ED2EE8FEFD}" type="CELLRANGE">
+                    <a:fld id="{05699C45-D819-44A3-A28C-0806F90C731A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3491,7 +3491,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9719D1E8-37E7-4C36-A739-570C1FB29C94}" type="CELLRANGE">
+                    <a:fld id="{0F8CEFFA-5CF1-420B-882C-205BE22194BC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3524,7 +3524,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{67D25AED-E001-4F6B-93E7-5DE5FC39AF2E}" type="CELLRANGE">
+                    <a:fld id="{4E084D62-E2FD-4F5D-8EAB-2F5D874CC896}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3557,7 +3557,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2BBDBE01-58F3-4669-AEC2-97733BE67DAF}" type="CELLRANGE">
+                    <a:fld id="{BF211231-5CE4-496A-AF0F-5124EEC6F0DE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3590,7 +3590,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9717DEEC-9372-4727-987D-75DBF0D98CBD}" type="CELLRANGE">
+                    <a:fld id="{27A50454-FF35-4E03-AC17-05CDB40F0E6A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20065,7 +20065,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -20131,7 +20131,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="E1:F6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" subtotalTop="0" showAll="0">
@@ -20183,7 +20183,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H2:I8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -20268,7 +20268,7 @@
     <tableColumn id="9" name="vote3"/>
     <tableColumn id="10" name="vote4"/>
     <tableColumn id="11" name="vote5"/>
-    <tableColumn id="12" name="data_type" dataDxfId="0">
+    <tableColumn id="12" name="data_type" dataDxfId="13">
       <calculatedColumnFormula>IF(ISNA(VLOOKUP(Table1[[#This Row],[loc]],val_dataset!$A$168:$B$208,2,FALSE)),"train","val")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -20277,33 +20277,33 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:K141" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:K141" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11">
   <autoFilter ref="A1:K141"/>
   <sortState ref="A2:K141">
     <sortCondition descending="1" ref="K1:K141"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" name="img_id" dataDxfId="11"/>
-    <tableColumn id="2" name="1" dataDxfId="10"/>
-    <tableColumn id="3" name="2" dataDxfId="9"/>
-    <tableColumn id="4" name="3" dataDxfId="8"/>
-    <tableColumn id="5" name="4" dataDxfId="7"/>
-    <tableColumn id="6" name="5" dataDxfId="6">
+    <tableColumn id="1" name="img_id" dataDxfId="10"/>
+    <tableColumn id="2" name="1" dataDxfId="9"/>
+    <tableColumn id="3" name="2" dataDxfId="8"/>
+    <tableColumn id="4" name="3" dataDxfId="7"/>
+    <tableColumn id="5" name="4" dataDxfId="6"/>
+    <tableColumn id="6" name="5" dataDxfId="5">
       <calculatedColumnFormula>_xlfn.VAR.P(Table2[[#This Row],[1]:[4]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="dist1" dataDxfId="5">
+    <tableColumn id="7" name="dist1" dataDxfId="4">
       <calculatedColumnFormula>ABS(Table2[[#This Row],[1]]-Table2[[#This Row],[2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="dist2" dataDxfId="4">
+    <tableColumn id="8" name="dist2" dataDxfId="3">
       <calculatedColumnFormula>ABS(Table2[[#This Row],[2]]-Table2[[#This Row],[3]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="dist3" dataDxfId="3">
+    <tableColumn id="9" name="dist3" dataDxfId="2">
       <calculatedColumnFormula>ABS(Table2[[#This Row],[3]]-Table2[[#This Row],[4]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="dist4" dataDxfId="2">
+    <tableColumn id="10" name="dist4" dataDxfId="1">
       <calculatedColumnFormula>ABS(Table2[[#This Row],[4]]-Table2[[#This Row],[1]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="tot_dist" dataDxfId="1">
+    <tableColumn id="11" name="tot_dist" dataDxfId="0">
       <calculatedColumnFormula>SUM(Table2[[#This Row],[dist1]:[dist4]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -20701,8 +20701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M806"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60769,8 +60769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="H146" sqref="H146"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64545,8 +64545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P806"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64565,6 +64565,10 @@
       </c>
       <c r="C2" t="s">
         <v>834</v>
+      </c>
+      <c r="N2">
+        <f>153/805</f>
+        <v>0.19006211180124225</v>
       </c>
       <c r="P2">
         <v>0</v>

</xml_diff>